<commit_message>
Added analog i/o calibration data, after correction
</commit_message>
<xml_diff>
--- a/res/analog_io_calibration.xlsx
+++ b/res/analog_io_calibration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27465" windowHeight="11265" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27465" windowHeight="11265"/>
   </bookViews>
   <sheets>
     <sheet name="read" sheetId="1" r:id="rId1"/>
@@ -102,12 +102,84 @@
         </r>
       </text>
     </comment>
+    <comment ref="B60" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Craig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+dacWrite function</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C60" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Craig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+dacWrite function</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D60" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Craig:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ledCWrite function, with 8-bit resolution (255 max value) and 12kHz frequency</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>PR1</t>
   </si>
@@ -177,6 +249,15 @@
   <si>
     <t>Value passed to ledcWrite / maximum</t>
   </si>
+  <si>
+    <t>After correction based on polynomial fit:</t>
+  </si>
+  <si>
+    <t>Ideal</t>
+  </si>
+  <si>
+    <t>After calibration</t>
+  </si>
 </sst>
 </file>
 
@@ -232,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -247,6 +328,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1684,6 +1768,450 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>read!$B$52</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual voltage / maximum voltage</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:name>Linear fit with 0,0 intercept</c:name>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.03172027240464E-2"/>
+                  <c:y val="-4.2614101154975763E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>read!$A$53:$A$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>255</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>read!$B$53:$B$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-30A5-42D1-A6A5-3FC416CBAADA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="453293752"/>
+        <c:axId val="453289488"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="453293752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="453289488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="453289488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="453293752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2922,7 +3450,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3458,7 +3986,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3999,6 +4527,1266 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>analog write calibration</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>write!$B$59:$B$60</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Measured voltage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PR1 (dacWrite)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>write!$A$61:$A$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>write!$B$61:$B$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.53</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.99</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.46</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.46</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.96</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.53</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.9400000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8734-420A-86FC-A591E3CB93F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>write!$C$59:$C$60</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Measured voltage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PR2 (dacWrite)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>write!$A$61:$A$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>write!$C$61:$C$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.91</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.41</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.92</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.9400000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8734-420A-86FC-A591E3CB93F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>write!$D$59:$D$60</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Measured voltage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PR3 (ledCWrite)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>write!$A$61:$A$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>write!$D$61:$D$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.97</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.93</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.43</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.96</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.9400000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8734-420A-86FC-A591E3CB93F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>write!$E$59:$E$60</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Measured voltage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ideal (linear)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>write!$A$61:$A$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>write!$E$61:$E$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8734-420A-86FC-A591E3CB93F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="11956592"/>
+        <c:axId val="11956920"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>write!$A$59:$A$60</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>Requested voltage</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>write!$A$61:$A$71</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="11"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.5</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2.5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>3.5</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>4.5</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>5</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>write!$A$61:$A$71</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="11"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.5</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2.5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>3.5</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>4.5</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>5</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-8734-420A-86FC-A591E3CB93F4}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="5"/>
+                <c:order val="5"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>write!$F$59:$F$60</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>Measured voltage</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>dacWrite average</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent6"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>write!$A$61:$A$71</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="11"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.5</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2.5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>3.5</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>4.5</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>5</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>write!$F$61:$F$71</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="11"/>
+                      <c:pt idx="0">
+                        <c:v>0.1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.0249999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.5150000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1.9750000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2.4450000000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2.93</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>3.4350000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>3.94</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>4.5150000000000006</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>4.9400000000000004</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000005-8734-420A-86FC-A591E3CB93F4}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="11956592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Requested voltage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="11956920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="11956920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Measured voltage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="11956592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4199,6 +5987,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -5219,7 +7087,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5246,8 +7114,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5348,7 +7216,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -5380,10 +7248,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -5423,22 +7291,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -5543,8 +7412,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5676,19 +7545,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -5702,6 +7572,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -5722,7 +7603,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5749,8 +7630,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5851,7 +7732,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -5883,10 +7764,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -5926,23 +7807,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -6047,8 +7927,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6180,20 +8060,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -6207,17 +8086,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -6734,6 +8602,1025 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -6810,6 +9697,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6909,6 +9828,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7180,15 +10131,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="V59" sqref="V59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="66" customHeight="1" x14ac:dyDescent="0.25">
@@ -7638,6 +10590,154 @@
         <v>1</v>
       </c>
     </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>4</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <f>255*B53</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>22</v>
+      </c>
+      <c r="B54">
+        <v>0.1</v>
+      </c>
+      <c r="C54">
+        <f t="shared" ref="C54:C63" si="2">255*B54</f>
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>51</v>
+      </c>
+      <c r="B55">
+        <v>0.2</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>79</v>
+      </c>
+      <c r="B56">
+        <v>0.3</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="2"/>
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>107</v>
+      </c>
+      <c r="B57">
+        <v>0.4</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="2"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>134</v>
+      </c>
+      <c r="B58">
+        <v>0.5</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="2"/>
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>160</v>
+      </c>
+      <c r="B59">
+        <v>0.6</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="2"/>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>183</v>
+      </c>
+      <c r="B60">
+        <v>0.7</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="2"/>
+        <v>178.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>208</v>
+      </c>
+      <c r="B61">
+        <v>0.8</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="2"/>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>235</v>
+      </c>
+      <c r="B62">
+        <v>0.9</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="2"/>
+        <v>229.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>255</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:D2"/>
@@ -7652,10 +10752,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R52"/>
+  <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="S52" sqref="S52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7969,7 +11069,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" ref="A24:A35" si="1">F5/4.94</f>
+        <f t="shared" ref="A24:A33" si="1">F5/4.94</f>
         <v>0.12145748987854249</v>
       </c>
       <c r="B24">
@@ -8150,7 +11250,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="3"/>
         <v>0.76720647773279349</v>
@@ -8160,7 +11260,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="3"/>
         <v>0.88056680161943301</v>
@@ -8170,7 +11270,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="3"/>
         <v>0.98785425101214563</v>
@@ -8180,7 +11280,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -8190,11 +11290,277 @@
         <v>1</v>
       </c>
     </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="6"/>
+      <c r="B60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>0</v>
+      </c>
+      <c r="B61">
+        <v>0.12</v>
+      </c>
+      <c r="C61">
+        <v>0.08</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <f>AVERAGE(B61:C61)</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>0.5</v>
+      </c>
+      <c r="B62">
+        <v>0.52</v>
+      </c>
+      <c r="C62">
+        <v>0.48</v>
+      </c>
+      <c r="D62">
+        <v>0.52</v>
+      </c>
+      <c r="E62">
+        <v>0.5</v>
+      </c>
+      <c r="F62">
+        <f t="shared" ref="F62:F71" si="5">AVERAGE(B62:C62)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>1.05</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>1.03</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="5"/>
+        <v>1.0249999999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1.5</v>
+      </c>
+      <c r="B64">
+        <v>1.53</v>
+      </c>
+      <c r="C64">
+        <v>1.5</v>
+      </c>
+      <c r="D64">
+        <v>1.5</v>
+      </c>
+      <c r="E64">
+        <v>1.5</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="5"/>
+        <v>1.5150000000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>2</v>
+      </c>
+      <c r="B65">
+        <v>1.99</v>
+      </c>
+      <c r="C65">
+        <v>1.96</v>
+      </c>
+      <c r="D65">
+        <v>1.97</v>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="5"/>
+        <v>1.9750000000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>2.5</v>
+      </c>
+      <c r="B66">
+        <v>2.46</v>
+      </c>
+      <c r="C66">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="D66">
+        <v>2.44</v>
+      </c>
+      <c r="E66">
+        <v>2.5</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="5"/>
+        <v>2.4450000000000003</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>3</v>
+      </c>
+      <c r="B67">
+        <v>2.95</v>
+      </c>
+      <c r="C67">
+        <v>2.91</v>
+      </c>
+      <c r="D67">
+        <v>2.93</v>
+      </c>
+      <c r="E67">
+        <v>3</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="5"/>
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>3.5</v>
+      </c>
+      <c r="B68">
+        <v>3.46</v>
+      </c>
+      <c r="C68">
+        <v>3.41</v>
+      </c>
+      <c r="D68">
+        <v>3.43</v>
+      </c>
+      <c r="E68">
+        <v>3.5</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="5"/>
+        <v>3.4350000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>4</v>
+      </c>
+      <c r="B69">
+        <v>3.96</v>
+      </c>
+      <c r="C69">
+        <v>3.92</v>
+      </c>
+      <c r="D69">
+        <v>3.96</v>
+      </c>
+      <c r="E69">
+        <v>4</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="5"/>
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>4.5</v>
+      </c>
+      <c r="B70">
+        <v>4.53</v>
+      </c>
+      <c r="C70">
+        <v>4.5</v>
+      </c>
+      <c r="D70">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="E70">
+        <v>4.5</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="5"/>
+        <v>4.5150000000000006</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>5</v>
+      </c>
+      <c r="B71">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="C71">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="D71">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="E71">
+        <v>5</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="5"/>
+        <v>4.9400000000000004</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="B59:D59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>